<commit_message>
colour temp and calibration
</commit_message>
<xml_diff>
--- a/Year_3/spectroscopy/data/Merc_Lamp.xlsx
+++ b/Year_3/spectroscopy/data/Merc_Lamp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\campus.gla.ac.uk\isi\stud-file\My Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewis\Document\Github\Physics\Year_3\spectroscopy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD9EB21-E459-4D93-9189-06EC49F5B2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB2C1AC-BCB6-4C40-9A01-666BB10E0C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{F6E535C2-DE44-4999-B61D-FE9DCBFB0192}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="3" xr2:uid="{F6E535C2-DE44-4999-B61D-FE9DCBFB0192}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -18,46 +18,25 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="2">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
         </ext>
       </extLst>
     </bk>
@@ -67,16 +46,11 @@
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="2" v="0"/>
-    </bk>
-  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
   <si>
     <t>Wavelengths (nm)</t>
   </si>
@@ -179,6 +153,9 @@
   <si>
     <t>X Variable 3</t>
   </si>
+  <si>
+    <t>wave diff nm</t>
+  </si>
 </sst>
 </file>
 
@@ -246,14 +223,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2371,16 +2347,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1533525</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:colOff>1266825</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2407,16 +2383,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1533525</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1057275</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2816,48 +2792,48 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:9">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>5</v>
       </c>
     </row>
@@ -2867,156 +2843,154 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>33949.199999999997</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>33949.199999999997</v>
       </c>
-      <c r="E12" s="1" t="e">
+      <c r="E12" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="F12" s="1" t="e">
+      <c r="F12" t="e">
         <v>#NUM!</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>3</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>4</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>33949.199999999997</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="16" spans="1:9">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>350</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>65535</v>
       </c>
-      <c r="E17" s="1" t="e">
+      <c r="E17" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
         <v>350</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17">
         <v>350</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17">
         <v>350</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17">
         <v>350</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>1</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>0</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>65535</v>
       </c>
-      <c r="E18" s="2" t="e">
+      <c r="E18" s="1" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>1</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <v>1</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1">
         <v>1</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="1">
         <v>1</v>
       </c>
     </row>
@@ -3043,48 +3017,48 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:9">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>5</v>
       </c>
     </row>
@@ -3094,214 +3068,212 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>3</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>33949.199999999997</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>11316.4</v>
       </c>
-      <c r="E12" s="1" t="e">
+      <c r="E12" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="F12" s="1" t="e">
+      <c r="F12" t="e">
         <v>#NUM!</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>4</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>33949.199999999997</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="16" spans="1:9">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>350</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>65535</v>
       </c>
-      <c r="E17" s="1" t="e">
+      <c r="E17" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
         <v>350</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17">
         <v>350</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17">
         <v>350</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17">
         <v>350</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>0</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>65535</v>
       </c>
-      <c r="E18" s="1" t="e">
+      <c r="E18" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18">
         <v>1</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18">
         <v>1</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18">
         <v>1</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>0</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>0</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>65535</v>
       </c>
-      <c r="E19" s="1" t="e">
+      <c r="E19" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>0</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19">
         <v>0</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19">
         <v>0</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>0</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>0</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>65535</v>
       </c>
-      <c r="E20" s="2" t="e">
+      <c r="E20" s="1" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>0</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>0</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="1">
         <v>0</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3327,51 +3299,51 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:9">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="I3" s="5">
+      <c r="B3" s="3"/>
+      <c r="I3" s="4">
         <v>376.47416827000001</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>0.99984104958305209</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>0.9996821244313393</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>0.99872849772535721</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>3.20859419844383</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>5</v>
       </c>
     </row>
@@ -3381,236 +3353,238 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>3</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>32376.832923269725</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>10792.277641089908</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
         <v>1048.2950174950881</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12">
         <v>2.2699468234536363E-2</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>10.295076730287404</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>10.295076730287404</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>4</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>32387.128000000012</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="16" spans="1:9">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>352.89713745172099</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>5.1380714443794995</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>68.682800788562915</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17">
         <v>9.268328988946915E-3</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
         <v>287.61174973034207</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17">
         <v>418.18252517309969</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17">
         <v>287.61174973034207</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17">
         <v>418.18252517309969</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>0.70739728081148301</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>0.19589513389202556</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>3.6111018520827072</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18">
         <v>0.17198528833675389</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18">
         <v>-1.7816863972409502</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18">
         <v>3.1964809588639174</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18">
         <v>-1.7816863972409502</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18">
         <v>3.1964809588639174</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>3.9870646802255003E-3</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>2.0606114247503607E-3</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>1.9348939990995746</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19">
         <v>0.3036779339789471</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>-2.2195485964353244E-2</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19">
         <v>3.0169615324804243E-2</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19">
         <v>-2.2195485964353244E-2</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19">
         <v>3.0169615324804243E-2</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="2" t="e" cm="1" vm="1">
-        <f t="array" ref="B20:B24">-Sheet1!E3:E7+Sheet1!E3:E7+Sheet1!F3:F7+Sheet1!F3:F7+Sheet1!F3:F7+_FV(Sheet1!I3376,"47416827")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B20" s="1" t="e" cm="1">
+        <f t="array" aca="1" ref="B20:B24" ca="1">-Sheet1!E3:E7+Sheet1!E3:E7+Sheet1!F3:F7+Sheet1!F3:F7+Sheet1!F3:F7+_FV(Sheet1!I3376,"47416827")</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C20" s="1">
         <v>5.9802269641034311E-6</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>-2.1741026341245941</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>0.27445036932619166</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>-8.8987615370010896E-5</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>6.2984360979370505E-5</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="1">
         <v>-8.8987615370010896E-5</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="1">
         <v>6.2984360979370505E-5</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="B21" t="e" vm="1">
-        <v>#VALUE!</v>
+      <c r="B21" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="B22" t="e" vm="1">
-        <v>#VALUE!</v>
+      <c r="B22" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="B23" t="e" vm="1">
-        <v>#VALUE!</v>
+      <c r="B23" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="B24" t="e" vm="1">
-        <v>#VALUE!</v>
+      <c r="B24" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
@@ -3620,15 +3594,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3571E9A4-85D2-4FC1-90F5-4651DB0C309D}">
-  <dimension ref="A1:I652"/>
+  <dimension ref="A1:J652"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.28515625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3636,7 +3610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>350</v>
       </c>
@@ -3658,8 +3632,11 @@
       <c r="I2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>351</v>
       </c>
@@ -3683,8 +3660,12 @@
       <c r="I3">
         <v>376.47416827000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <f>(I3-E3)</f>
+        <v>11.464168270000016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>352</v>
       </c>
@@ -3705,11 +3686,15 @@
         <f t="shared" ref="H4:H7" si="1">(F4^3)</f>
         <v>157464</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>446.16844555</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <f t="shared" ref="J4:J7" si="2">(I4-E4)</f>
+        <v>47.778445550000015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>353</v>
       </c>
@@ -3730,11 +3715,15 @@
         <f t="shared" si="1"/>
         <v>614125</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>516.78068687999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>80.950686879999978</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>354</v>
       </c>
@@ -3755,11 +3744,15 @@
         <f t="shared" si="1"/>
         <v>7529536</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>739.99072377000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>193.92072377</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>355</v>
       </c>
@@ -3780,11 +3773,15 @@
         <f t="shared" si="1"/>
         <v>11852352</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>782.20028826999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>214.45028826999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>356</v>
       </c>
@@ -3792,7 +3789,7 @@
         <v>225.67</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>357</v>
       </c>
@@ -3800,7 +3797,7 @@
         <v>234.99</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>358</v>
       </c>
@@ -3808,7 +3805,7 @@
         <v>234.25</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>359</v>
       </c>
@@ -3816,7 +3813,7 @@
         <v>234.67</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>360</v>
       </c>
@@ -3824,7 +3821,7 @@
         <v>244.89</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>361</v>
       </c>
@@ -3832,7 +3829,7 @@
         <v>271.64</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>362</v>
       </c>
@@ -3840,7 +3837,7 @@
         <v>408.33</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>363</v>
       </c>
@@ -3848,7 +3845,7 @@
         <v>2006.63</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>364</v>
       </c>
@@ -8946,6 +8943,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>